<commit_message>
Updated and Added Open agent
</commit_message>
<xml_diff>
--- a/Output_Nab.xlsx
+++ b/Output_Nab.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <x:si>
     <x:t>Address</x:t>
   </x:si>
   <x:si>
+    <x:t>ExtractedAddress</x:t>
+  </x:si>
+  <x:si>
     <x:t>LowPrice</x:t>
   </x:si>
   <x:si>
@@ -31,28 +34,373 @@
     <x:t>Status</x:t>
   </x:si>
   <x:si>
-    <x:t>15 GARIBALDI STREET TRARALGON VIC 3844</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$417K</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$345K</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$470K</x:t>
+    <x:t>3 newcastle street thornbury vic 3071</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.6m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.86m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$2.12m</x:t>
   </x:si>
   <x:si>
     <x:t>Successful</x:t>
   </x:si>
   <x:si>
-    <x:t>57 WARWICK STREET CLEARVIEW SA 5085</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Address not Found</x:t>
+    <x:t>30 nelley way wickham wa 6720</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$325k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$380k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$435k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28 acacia way wallan vic 3756</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$430k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$500k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$570k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4 riverglen drive werribee vic 3030</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$445k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$520k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$595k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>53 firestone way west wodonga vic 3690</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Price Missing</x:t>
   </x:si>
   <x:si>
     <x:t>Failed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20 loretta avenue wheelers hill vic 3150</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.07m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.24m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.41m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12 beardmore street wodonga vic 3690</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$175k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$205k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$235k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 whiteley circuit baranduda vic 3691</x:t>
+  </x:si>
+  <x:si>
+    <x:t>302/3018 surfers paradise boulevard surfers paradise qld 4217</x:t>
+  </x:si>
+  <x:si>
+    <x:t>118 alice street goodna qld 4300</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$250k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$295k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$340k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>119 bridge street north toowoomba qld 4350</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27 balmoral road kellyville nsw 2155</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.4m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.62m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.84m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>45 duncan street west end qld 4101</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Address Not Found</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6 parkes drive korora nsw 2450</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$780k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$910k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.04m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8 danbulla street pimpama qld 4209</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$365k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$420k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$475k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3/14-16 burrendong way orange nsw 2800</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$160k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$190k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$220k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2 kyla avenue dandenong vic 3175</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$675k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$885k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1/14 clara street east maitland nsw 2323</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$405k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$465k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$525k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>142/350 leitchs road brendale qld 4500</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$255k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$275k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>46c the promenade mount pleasant wa 6153</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26 kinsale parkway canning vale wa 6155</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17 solomon parade warner qld 4500</x:t>
+  </x:si>
+  <x:si>
+    <x:t>410/3 alma road macquarie park nsw 2113</x:t>
+  </x:si>
+  <x:si>
+    <x:t>89 bay park road wondunna qld 4655</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$285k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$335k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$385k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4/17 denbigh place south nowra nsw 2541</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$350k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$460k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8 st andrews drive leichhardt qld 4305</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3/1a lyndhurst street richmond vic 3121</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33 summerhill crescent ormeau hills qld 4208</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$375k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$440k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$505k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24 dorset street haynes wa 6112</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$310k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$360k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$410k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15 the heights hillvue nsw 2340</x:t>
+  </x:si>
+  <x:si>
+    <x:t>60/36 queen victoria street fremantle wa 6160</x:t>
+  </x:si>
+  <x:si>
+    <x:t>136b merrigang street bowral nsw 2576</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.47m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.7m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$1.93m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>146-148 panitz drive jimboomba qld 4280</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$590k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>54 sienna circuit yarrabilba qld 4207</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$415k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20 woodleigh way harrisdale wa 6112</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$540k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$620k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1/10 buss street bundaberg south qld 4670</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$215k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10 biara gardens mount claremont wa 6010</x:t>
+  </x:si>
+  <x:si>
+    <x:t>71a benara road noranda wa 6062</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24 binda avenue springvale vic 3171</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$635k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$740k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$845k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13 caladenia street deebing heights qld 4306</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$390k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$425k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15/41-45 south street rydalmere nsw 2116</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$490k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$650k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2/37 charles street st albans vic 3021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$485k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$555k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47 firmstone road leneva vic 3691</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7 mckinley road hilbert wa 6112</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25 magiltan drive strathbogie vic 3666</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13 banjolina circuit craigieburn vic 3064</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$745k</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 lakes crescent south yunderup wa 6208</x:t>
+  </x:si>
+  <x:si>
+    <x:t>105/151-153 huntingdale road ashwood vic 3147</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16a tindall court alligator creek qld 4816</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1005/145 queensberry street carlton vic 3053</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -409,7 +757,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -425,12 +773,12 @@
       <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5">
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
@@ -442,22 +790,841 @@
       <x:c r="E2" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5">
+      <x:c r="F2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
+      <x:c r="A6" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="A7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="A8" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="A9" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="A12" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="A13" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="A15" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="A17" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="A18" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="A20" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="A21" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="A24" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="A25" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="A26" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="A29" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="A30" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="A31" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="A32" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="A33" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="A34" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="A37" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="F37" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="A38" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F38" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="A39" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F39" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="A40" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>108</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>109</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="F40" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="A41" s="0" t="s">
+        <x:v>111</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>112</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>113</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:6">
+      <x:c r="A42" s="0" t="s">
+        <x:v>114</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>115</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E42" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="F42" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:6">
+      <x:c r="A43" s="0" t="s">
+        <x:v>117</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>118</x:v>
+      </x:c>
+      <x:c r="E43" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="F43" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:6">
+      <x:c r="A44" s="0" t="s">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E44" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F44" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:6">
+      <x:c r="A45" s="0" t="s">
+        <x:v>121</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F45" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:6">
+      <x:c r="A46" s="0" t="s">
+        <x:v>122</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E46" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F46" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:6">
+      <x:c r="A47" s="0" t="s">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>119</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>116</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="s">
+        <x:v>124</x:v>
+      </x:c>
+      <x:c r="F47" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:6">
+      <x:c r="A48" s="0" t="s">
+        <x:v>125</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="E48" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F48" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:6">
+      <x:c r="A49" s="0" t="s">
+        <x:v>126</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E49" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F49" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:6">
+      <x:c r="A50" s="0" t="s">
+        <x:v>127</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E50" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F50" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:6">
+      <x:c r="A51" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F51" s="0" t="s">
+        <x:v>25</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>